<commit_message>
Display AA now working Incomplete data fixed
</commit_message>
<xml_diff>
--- a/RDS Agreement Manager.xlsx
+++ b/RDS Agreement Manager.xlsx
@@ -2,17 +2,36 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="ContractType">Main!$F$2</definedName>
+    <definedName name="CrewName">Main!$C$2</definedName>
+    <definedName name="CrewNo">Main!$B$3</definedName>
+    <definedName name="HrsWk">Main!$G$2</definedName>
+    <definedName name="NoWeeks">Main!$H$2</definedName>
+    <definedName name="RevDate">Main!$I$2</definedName>
+    <definedName name="Role">Main!$D$2</definedName>
+    <definedName name="SlotStart">Main!$B$4</definedName>
+    <definedName name="TemplateDate">Main!$E$2</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>CrewNo</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,18 +368,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr codeName="ShtFrontPage"/>
+  <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -373,6 +402,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Work on Agreement Class Further DB changes
</commit_message>
<xml_diff>
--- a/RDS Agreement Manager.xlsx
+++ b/RDS Agreement Manager.xlsx
@@ -29,12 +29,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Julian Turner</t>
+    <t>Over 120 Hrs</t>
   </si>
   <si>
-    <t>CM</t>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Alan Maskell</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>EC16 - Horncastle</t>
   </si>
 </sst>
 </file>
@@ -175,6 +184,56 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>49</xdr:col>
+          <xdr:colOff>466725</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>50</xdr:col>
+          <xdr:colOff>1295400</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="ComboBox1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -463,338 +522,323 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtFrontPage"/>
-  <dimension ref="B2:AW98"/>
+  <dimension ref="B2:AY98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ20" sqref="AJ20"/>
+      <selection activeCell="BA12" sqref="BA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="49" width="3.140625" customWidth="1"/>
+    <col min="2" max="49" width="2.5703125" customWidth="1"/>
+    <col min="51" max="51" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>5398</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>42675</v>
-      </c>
-      <c r="F2">
+    <row r="2" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="4" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="4">
+        <v>0</v>
+      </c>
+      <c r="X4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AU4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AY4">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="5" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7">
+        <v>1</v>
+      </c>
+      <c r="P5" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7">
+        <v>1</v>
+      </c>
+      <c r="S5" s="7">
+        <v>1</v>
+      </c>
+      <c r="T5" s="7">
+        <v>1</v>
+      </c>
+      <c r="U5" s="7">
+        <v>1</v>
+      </c>
+      <c r="V5" s="7">
+        <v>1</v>
+      </c>
+      <c r="W5" s="7">
+        <v>1</v>
+      </c>
+      <c r="X5" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AY5" t="s">
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>124</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="4">
-        <v>1</v>
-      </c>
-      <c r="O4" s="4">
-        <v>1</v>
-      </c>
-      <c r="P4" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>1</v>
-      </c>
-      <c r="R4" s="4">
-        <v>1</v>
-      </c>
-      <c r="S4" s="4">
-        <v>1</v>
-      </c>
-      <c r="T4" s="4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="4">
-        <v>0</v>
-      </c>
-      <c r="V4" s="4">
-        <v>0</v>
-      </c>
-      <c r="W4" s="4">
-        <v>0</v>
-      </c>
-      <c r="X4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AP4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AR4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AS4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AT4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AU4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AV4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AW4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1</v>
-      </c>
-      <c r="J5" s="7">
-        <v>1</v>
-      </c>
-      <c r="K5" s="7">
-        <v>1</v>
-      </c>
-      <c r="L5" s="7">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>1</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1</v>
-      </c>
-      <c r="P5" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>1</v>
-      </c>
-      <c r="R5" s="7">
-        <v>1</v>
-      </c>
-      <c r="S5" s="7">
-        <v>1</v>
-      </c>
-      <c r="T5" s="7">
-        <v>0</v>
-      </c>
-      <c r="U5" s="7">
-        <v>0</v>
-      </c>
-      <c r="V5" s="7">
-        <v>0</v>
-      </c>
-      <c r="W5" s="7">
-        <v>0</v>
-      </c>
-      <c r="X5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AM5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AO5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AP5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AT5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AU5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AV5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:49" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>1</v>
       </c>
@@ -850,52 +894,52 @@
         <v>1</v>
       </c>
       <c r="T6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6" s="7">
         <v>1</v>
@@ -939,8 +983,11 @@
       <c r="AW6" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AY6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>1</v>
       </c>
@@ -987,13 +1034,13 @@
         <v>1</v>
       </c>
       <c r="Q7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" s="7">
         <v>0</v>
@@ -1044,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="7">
         <v>1</v>
@@ -1085,8 +1132,11 @@
       <c r="AW7" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AY7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>1</v>
       </c>
@@ -1133,13 +1183,13 @@
         <v>1</v>
       </c>
       <c r="Q8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="7">
         <v>0</v>
@@ -1190,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="7">
         <v>1</v>
@@ -1231,8 +1281,11 @@
       <c r="AW8" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AY8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>1</v>
       </c>
@@ -1279,64 +1332,64 @@
         <v>1</v>
       </c>
       <c r="Q9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK9" s="7">
         <v>1</v>
@@ -1377,8 +1430,11 @@
       <c r="AW9" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AY9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>1</v>
       </c>
@@ -1425,64 +1481,64 @@
         <v>1</v>
       </c>
       <c r="Q10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ10" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK10" s="10">
         <v>1</v>
@@ -1523,8 +1579,16 @@
       <c r="AW10" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AY10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="AY11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>1</v>
       </c>
@@ -1571,13 +1635,13 @@
         <v>1</v>
       </c>
       <c r="Q12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="4">
         <v>0</v>
@@ -1628,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK12" s="4">
         <v>1</v>
@@ -1669,8 +1733,11 @@
       <c r="AW12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AY12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>1</v>
       </c>
@@ -1726,52 +1793,52 @@
         <v>1</v>
       </c>
       <c r="T13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ13" s="7">
         <v>1</v>
@@ -1815,8 +1882,11 @@
       <c r="AW13" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AY13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>1</v>
       </c>
@@ -1872,52 +1942,52 @@
         <v>1</v>
       </c>
       <c r="T14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14" s="7">
         <v>1</v>
@@ -1962,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>1</v>
       </c>
@@ -2009,13 +2079,13 @@
         <v>1</v>
       </c>
       <c r="Q15" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="7">
         <v>0</v>
@@ -2066,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK15" s="7">
         <v>1</v>
@@ -2108,7 +2178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>1</v>
       </c>
@@ -2155,13 +2225,13 @@
         <v>1</v>
       </c>
       <c r="Q16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="7">
         <v>0</v>
@@ -2212,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="AJ16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK16" s="7">
         <v>1</v>
@@ -2486,46 +2556,46 @@
         <v>1</v>
       </c>
       <c r="AD18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR18" s="10">
         <v>1</v>
@@ -2547,704 +2617,2048 @@
       </c>
     </row>
     <row r="20" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
-      <c r="AD20" s="4"/>
-      <c r="AE20" s="4"/>
-      <c r="AF20" s="4"/>
-      <c r="AG20" s="4"/>
-      <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
-      <c r="AJ20" s="4"/>
-      <c r="AK20" s="4"/>
-      <c r="AL20" s="4"/>
-      <c r="AM20" s="4"/>
-      <c r="AN20" s="4"/>
-      <c r="AO20" s="4"/>
-      <c r="AP20" s="4"/>
-      <c r="AQ20" s="4"/>
-      <c r="AR20" s="4"/>
-      <c r="AS20" s="4"/>
-      <c r="AT20" s="4"/>
-      <c r="AU20" s="4"/>
-      <c r="AV20" s="4"/>
-      <c r="AW20" s="5"/>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1</v>
+      </c>
+      <c r="O20" s="4">
+        <v>1</v>
+      </c>
+      <c r="P20" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>0</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <v>0</v>
+      </c>
+      <c r="T20" s="4">
+        <v>0</v>
+      </c>
+      <c r="U20" s="4">
+        <v>0</v>
+      </c>
+      <c r="V20" s="4">
+        <v>0</v>
+      </c>
+      <c r="W20" s="4">
+        <v>0</v>
+      </c>
+      <c r="X20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AU20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AV20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW20" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-      <c r="AB21" s="7"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
-      <c r="AI21" s="7"/>
-      <c r="AJ21" s="7"/>
-      <c r="AK21" s="7"/>
-      <c r="AL21" s="7"/>
-      <c r="AM21" s="7"/>
-      <c r="AN21" s="7"/>
-      <c r="AO21" s="7"/>
-      <c r="AP21" s="7"/>
-      <c r="AQ21" s="7"/>
-      <c r="AR21" s="7"/>
-      <c r="AS21" s="7"/>
-      <c r="AT21" s="7"/>
-      <c r="AU21" s="7"/>
-      <c r="AV21" s="7"/>
-      <c r="AW21" s="8"/>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7">
+        <v>1</v>
+      </c>
+      <c r="I21" s="7">
+        <v>1</v>
+      </c>
+      <c r="J21" s="7">
+        <v>1</v>
+      </c>
+      <c r="K21" s="7">
+        <v>1</v>
+      </c>
+      <c r="L21" s="7">
+        <v>1</v>
+      </c>
+      <c r="M21" s="7">
+        <v>1</v>
+      </c>
+      <c r="N21" s="7">
+        <v>1</v>
+      </c>
+      <c r="O21" s="7">
+        <v>1</v>
+      </c>
+      <c r="P21" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0</v>
+      </c>
+      <c r="R21" s="7">
+        <v>0</v>
+      </c>
+      <c r="S21" s="7">
+        <v>0</v>
+      </c>
+      <c r="T21" s="7">
+        <v>0</v>
+      </c>
+      <c r="U21" s="7">
+        <v>0</v>
+      </c>
+      <c r="V21" s="7">
+        <v>0</v>
+      </c>
+      <c r="W21" s="7">
+        <v>0</v>
+      </c>
+      <c r="X21" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW21" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
-      <c r="AA22" s="7"/>
-      <c r="AB22" s="7"/>
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
-      <c r="AF22" s="7"/>
-      <c r="AG22" s="7"/>
-      <c r="AH22" s="7"/>
-      <c r="AI22" s="7"/>
-      <c r="AJ22" s="7"/>
-      <c r="AK22" s="7"/>
-      <c r="AL22" s="7"/>
-      <c r="AM22" s="7"/>
-      <c r="AN22" s="7"/>
-      <c r="AO22" s="7"/>
-      <c r="AP22" s="7"/>
-      <c r="AQ22" s="7"/>
-      <c r="AR22" s="7"/>
-      <c r="AS22" s="7"/>
-      <c r="AT22" s="7"/>
-      <c r="AU22" s="7"/>
-      <c r="AV22" s="7"/>
-      <c r="AW22" s="8"/>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7">
+        <v>1</v>
+      </c>
+      <c r="I22" s="7">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7">
+        <v>1</v>
+      </c>
+      <c r="K22" s="7">
+        <v>1</v>
+      </c>
+      <c r="L22" s="7">
+        <v>1</v>
+      </c>
+      <c r="M22" s="7">
+        <v>1</v>
+      </c>
+      <c r="N22" s="7">
+        <v>1</v>
+      </c>
+      <c r="O22" s="7">
+        <v>1</v>
+      </c>
+      <c r="P22" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>0</v>
+      </c>
+      <c r="R22" s="7">
+        <v>0</v>
+      </c>
+      <c r="S22" s="7">
+        <v>0</v>
+      </c>
+      <c r="T22" s="7">
+        <v>0</v>
+      </c>
+      <c r="U22" s="7">
+        <v>0</v>
+      </c>
+      <c r="V22" s="7">
+        <v>0</v>
+      </c>
+      <c r="W22" s="7">
+        <v>0</v>
+      </c>
+      <c r="X22" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV22" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW22" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="7"/>
-      <c r="AH23" s="7"/>
-      <c r="AI23" s="7"/>
-      <c r="AJ23" s="7"/>
-      <c r="AK23" s="7"/>
-      <c r="AL23" s="7"/>
-      <c r="AM23" s="7"/>
-      <c r="AN23" s="7"/>
-      <c r="AO23" s="7"/>
-      <c r="AP23" s="7"/>
-      <c r="AQ23" s="7"/>
-      <c r="AR23" s="7"/>
-      <c r="AS23" s="7"/>
-      <c r="AT23" s="7"/>
-      <c r="AU23" s="7"/>
-      <c r="AV23" s="7"/>
-      <c r="AW23" s="8"/>
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7">
+        <v>1</v>
+      </c>
+      <c r="J23" s="7">
+        <v>1</v>
+      </c>
+      <c r="K23" s="7">
+        <v>1</v>
+      </c>
+      <c r="L23" s="7">
+        <v>1</v>
+      </c>
+      <c r="M23" s="7">
+        <v>1</v>
+      </c>
+      <c r="N23" s="7">
+        <v>1</v>
+      </c>
+      <c r="O23" s="7">
+        <v>1</v>
+      </c>
+      <c r="P23" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>0</v>
+      </c>
+      <c r="R23" s="7">
+        <v>0</v>
+      </c>
+      <c r="S23" s="7">
+        <v>0</v>
+      </c>
+      <c r="T23" s="7">
+        <v>0</v>
+      </c>
+      <c r="U23" s="7">
+        <v>0</v>
+      </c>
+      <c r="V23" s="7">
+        <v>0</v>
+      </c>
+      <c r="W23" s="7">
+        <v>0</v>
+      </c>
+      <c r="X23" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW23" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
-      <c r="AJ24" s="7"/>
-      <c r="AK24" s="7"/>
-      <c r="AL24" s="7"/>
-      <c r="AM24" s="7"/>
-      <c r="AN24" s="7"/>
-      <c r="AO24" s="7"/>
-      <c r="AP24" s="7"/>
-      <c r="AQ24" s="7"/>
-      <c r="AR24" s="7"/>
-      <c r="AS24" s="7"/>
-      <c r="AT24" s="7"/>
-      <c r="AU24" s="7"/>
-      <c r="AV24" s="7"/>
-      <c r="AW24" s="8"/>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7">
+        <v>1</v>
+      </c>
+      <c r="I24" s="7">
+        <v>1</v>
+      </c>
+      <c r="J24" s="7">
+        <v>1</v>
+      </c>
+      <c r="K24" s="7">
+        <v>1</v>
+      </c>
+      <c r="L24" s="7">
+        <v>1</v>
+      </c>
+      <c r="M24" s="7">
+        <v>1</v>
+      </c>
+      <c r="N24" s="7">
+        <v>1</v>
+      </c>
+      <c r="O24" s="7">
+        <v>1</v>
+      </c>
+      <c r="P24" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>0</v>
+      </c>
+      <c r="R24" s="7">
+        <v>0</v>
+      </c>
+      <c r="S24" s="7">
+        <v>0</v>
+      </c>
+      <c r="T24" s="7">
+        <v>0</v>
+      </c>
+      <c r="U24" s="7">
+        <v>0</v>
+      </c>
+      <c r="V24" s="7">
+        <v>0</v>
+      </c>
+      <c r="W24" s="7">
+        <v>0</v>
+      </c>
+      <c r="X24" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV24" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW24" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="7"/>
-      <c r="Y25" s="7"/>
-      <c r="Z25" s="7"/>
-      <c r="AA25" s="7"/>
-      <c r="AB25" s="7"/>
-      <c r="AC25" s="7"/>
-      <c r="AD25" s="7"/>
-      <c r="AE25" s="7"/>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="7"/>
-      <c r="AH25" s="7"/>
-      <c r="AI25" s="7"/>
-      <c r="AJ25" s="7"/>
-      <c r="AK25" s="7"/>
-      <c r="AL25" s="7"/>
-      <c r="AM25" s="7"/>
-      <c r="AN25" s="7"/>
-      <c r="AO25" s="7"/>
-      <c r="AP25" s="7"/>
-      <c r="AQ25" s="7"/>
-      <c r="AR25" s="7"/>
-      <c r="AS25" s="7"/>
-      <c r="AT25" s="7"/>
-      <c r="AU25" s="7"/>
-      <c r="AV25" s="7"/>
-      <c r="AW25" s="8"/>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1</v>
+      </c>
+      <c r="H25" s="7">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7">
+        <v>1</v>
+      </c>
+      <c r="J25" s="7">
+        <v>1</v>
+      </c>
+      <c r="K25" s="7">
+        <v>1</v>
+      </c>
+      <c r="L25" s="7">
+        <v>1</v>
+      </c>
+      <c r="M25" s="7">
+        <v>1</v>
+      </c>
+      <c r="N25" s="7">
+        <v>1</v>
+      </c>
+      <c r="O25" s="7">
+        <v>1</v>
+      </c>
+      <c r="P25" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>1</v>
+      </c>
+      <c r="R25" s="7">
+        <v>1</v>
+      </c>
+      <c r="S25" s="7">
+        <v>1</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7">
+        <v>1</v>
+      </c>
+      <c r="V25" s="7">
+        <v>1</v>
+      </c>
+      <c r="W25" s="7">
+        <v>1</v>
+      </c>
+      <c r="X25" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AF25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AH25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AJ25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW25" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-      <c r="W26" s="10"/>
-      <c r="X26" s="10"/>
-      <c r="Y26" s="10"/>
-      <c r="Z26" s="10"/>
-      <c r="AA26" s="10"/>
-      <c r="AB26" s="10"/>
-      <c r="AC26" s="10"/>
-      <c r="AD26" s="10"/>
-      <c r="AE26" s="10"/>
-      <c r="AF26" s="10"/>
-      <c r="AG26" s="10"/>
-      <c r="AH26" s="10"/>
-      <c r="AI26" s="10"/>
-      <c r="AJ26" s="10"/>
-      <c r="AK26" s="10"/>
-      <c r="AL26" s="10"/>
-      <c r="AM26" s="10"/>
-      <c r="AN26" s="10"/>
-      <c r="AO26" s="10"/>
-      <c r="AP26" s="10"/>
-      <c r="AQ26" s="10"/>
-      <c r="AR26" s="10"/>
-      <c r="AS26" s="10"/>
-      <c r="AT26" s="10"/>
-      <c r="AU26" s="10"/>
-      <c r="AV26" s="10"/>
-      <c r="AW26" s="11"/>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+      <c r="G26" s="10">
+        <v>1</v>
+      </c>
+      <c r="H26" s="10">
+        <v>1</v>
+      </c>
+      <c r="I26" s="10">
+        <v>1</v>
+      </c>
+      <c r="J26" s="10">
+        <v>1</v>
+      </c>
+      <c r="K26" s="10">
+        <v>1</v>
+      </c>
+      <c r="L26" s="10">
+        <v>1</v>
+      </c>
+      <c r="M26" s="10">
+        <v>1</v>
+      </c>
+      <c r="N26" s="10">
+        <v>1</v>
+      </c>
+      <c r="O26" s="10">
+        <v>1</v>
+      </c>
+      <c r="P26" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>1</v>
+      </c>
+      <c r="R26" s="10">
+        <v>1</v>
+      </c>
+      <c r="S26" s="10">
+        <v>1</v>
+      </c>
+      <c r="T26" s="10">
+        <v>1</v>
+      </c>
+      <c r="U26" s="10">
+        <v>1</v>
+      </c>
+      <c r="V26" s="10">
+        <v>1</v>
+      </c>
+      <c r="W26" s="10">
+        <v>1</v>
+      </c>
+      <c r="X26" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AN26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AO26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AP26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AR26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AT26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AW26" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
-      <c r="AG28" s="4"/>
-      <c r="AH28" s="4"/>
-      <c r="AI28" s="4"/>
-      <c r="AJ28" s="4"/>
-      <c r="AK28" s="4"/>
-      <c r="AL28" s="4"/>
-      <c r="AM28" s="4"/>
-      <c r="AN28" s="4"/>
-      <c r="AO28" s="4"/>
-      <c r="AP28" s="4"/>
-      <c r="AQ28" s="4"/>
-      <c r="AR28" s="4"/>
-      <c r="AS28" s="4"/>
-      <c r="AT28" s="4"/>
-      <c r="AU28" s="4"/>
-      <c r="AV28" s="4"/>
-      <c r="AW28" s="5"/>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1</v>
+      </c>
+      <c r="J28" s="4">
+        <v>1</v>
+      </c>
+      <c r="K28" s="4">
+        <v>1</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="M28" s="4">
+        <v>1</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1</v>
+      </c>
+      <c r="O28" s="4">
+        <v>1</v>
+      </c>
+      <c r="P28" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>0</v>
+      </c>
+      <c r="R28" s="4">
+        <v>0</v>
+      </c>
+      <c r="S28" s="4">
+        <v>0</v>
+      </c>
+      <c r="T28" s="4">
+        <v>0</v>
+      </c>
+      <c r="U28" s="4">
+        <v>0</v>
+      </c>
+      <c r="V28" s="4">
+        <v>0</v>
+      </c>
+      <c r="W28" s="4">
+        <v>0</v>
+      </c>
+      <c r="X28" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AU28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AV28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW28" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
-      <c r="AA29" s="7"/>
-      <c r="AB29" s="7"/>
-      <c r="AC29" s="7"/>
-      <c r="AD29" s="7"/>
-      <c r="AE29" s="7"/>
-      <c r="AF29" s="7"/>
-      <c r="AG29" s="7"/>
-      <c r="AH29" s="7"/>
-      <c r="AI29" s="7"/>
-      <c r="AJ29" s="7"/>
-      <c r="AK29" s="7"/>
-      <c r="AL29" s="7"/>
-      <c r="AM29" s="7"/>
-      <c r="AN29" s="7"/>
-      <c r="AO29" s="7"/>
-      <c r="AP29" s="7"/>
-      <c r="AQ29" s="7"/>
-      <c r="AR29" s="7"/>
-      <c r="AS29" s="7"/>
-      <c r="AT29" s="7"/>
-      <c r="AU29" s="7"/>
-      <c r="AV29" s="7"/>
-      <c r="AW29" s="8"/>
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1</v>
+      </c>
+      <c r="I29" s="7">
+        <v>1</v>
+      </c>
+      <c r="J29" s="7">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1</v>
+      </c>
+      <c r="L29" s="7">
+        <v>1</v>
+      </c>
+      <c r="M29" s="7">
+        <v>1</v>
+      </c>
+      <c r="N29" s="7">
+        <v>1</v>
+      </c>
+      <c r="O29" s="7">
+        <v>1</v>
+      </c>
+      <c r="P29" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>0</v>
+      </c>
+      <c r="R29" s="7">
+        <v>0</v>
+      </c>
+      <c r="S29" s="7">
+        <v>0</v>
+      </c>
+      <c r="T29" s="7">
+        <v>0</v>
+      </c>
+      <c r="U29" s="7">
+        <v>0</v>
+      </c>
+      <c r="V29" s="7">
+        <v>0</v>
+      </c>
+      <c r="W29" s="7">
+        <v>0</v>
+      </c>
+      <c r="X29" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW29" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
-      <c r="W30" s="7"/>
-      <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="7"/>
-      <c r="AB30" s="7"/>
-      <c r="AC30" s="7"/>
-      <c r="AD30" s="7"/>
-      <c r="AE30" s="7"/>
-      <c r="AF30" s="7"/>
-      <c r="AG30" s="7"/>
-      <c r="AH30" s="7"/>
-      <c r="AI30" s="7"/>
-      <c r="AJ30" s="7"/>
-      <c r="AK30" s="7"/>
-      <c r="AL30" s="7"/>
-      <c r="AM30" s="7"/>
-      <c r="AN30" s="7"/>
-      <c r="AO30" s="7"/>
-      <c r="AP30" s="7"/>
-      <c r="AQ30" s="7"/>
-      <c r="AR30" s="7"/>
-      <c r="AS30" s="7"/>
-      <c r="AT30" s="7"/>
-      <c r="AU30" s="7"/>
-      <c r="AV30" s="7"/>
-      <c r="AW30" s="8"/>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7">
+        <v>1</v>
+      </c>
+      <c r="I30" s="7">
+        <v>1</v>
+      </c>
+      <c r="J30" s="7">
+        <v>1</v>
+      </c>
+      <c r="K30" s="7">
+        <v>1</v>
+      </c>
+      <c r="L30" s="7">
+        <v>1</v>
+      </c>
+      <c r="M30" s="7">
+        <v>1</v>
+      </c>
+      <c r="N30" s="7">
+        <v>1</v>
+      </c>
+      <c r="O30" s="7">
+        <v>1</v>
+      </c>
+      <c r="P30" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>0</v>
+      </c>
+      <c r="R30" s="7">
+        <v>0</v>
+      </c>
+      <c r="S30" s="7">
+        <v>0</v>
+      </c>
+      <c r="T30" s="7">
+        <v>0</v>
+      </c>
+      <c r="U30" s="7">
+        <v>0</v>
+      </c>
+      <c r="V30" s="7">
+        <v>0</v>
+      </c>
+      <c r="W30" s="7">
+        <v>0</v>
+      </c>
+      <c r="X30" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW30" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7"/>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7"/>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7"/>
-      <c r="AJ31" s="7"/>
-      <c r="AK31" s="7"/>
-      <c r="AL31" s="7"/>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="7"/>
-      <c r="AO31" s="7"/>
-      <c r="AP31" s="7"/>
-      <c r="AQ31" s="7"/>
-      <c r="AR31" s="7"/>
-      <c r="AS31" s="7"/>
-      <c r="AT31" s="7"/>
-      <c r="AU31" s="7"/>
-      <c r="AV31" s="7"/>
-      <c r="AW31" s="8"/>
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1</v>
+      </c>
+      <c r="H31" s="7">
+        <v>1</v>
+      </c>
+      <c r="I31" s="7">
+        <v>1</v>
+      </c>
+      <c r="J31" s="7">
+        <v>1</v>
+      </c>
+      <c r="K31" s="7">
+        <v>1</v>
+      </c>
+      <c r="L31" s="7">
+        <v>1</v>
+      </c>
+      <c r="M31" s="7">
+        <v>1</v>
+      </c>
+      <c r="N31" s="7">
+        <v>1</v>
+      </c>
+      <c r="O31" s="7">
+        <v>1</v>
+      </c>
+      <c r="P31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>0</v>
+      </c>
+      <c r="R31" s="7">
+        <v>0</v>
+      </c>
+      <c r="S31" s="7">
+        <v>0</v>
+      </c>
+      <c r="T31" s="7">
+        <v>0</v>
+      </c>
+      <c r="U31" s="7">
+        <v>0</v>
+      </c>
+      <c r="V31" s="7">
+        <v>0</v>
+      </c>
+      <c r="W31" s="7">
+        <v>0</v>
+      </c>
+      <c r="X31" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW31" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="7"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="7"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="7"/>
-      <c r="AH32" s="7"/>
-      <c r="AI32" s="7"/>
-      <c r="AJ32" s="7"/>
-      <c r="AK32" s="7"/>
-      <c r="AL32" s="7"/>
-      <c r="AM32" s="7"/>
-      <c r="AN32" s="7"/>
-      <c r="AO32" s="7"/>
-      <c r="AP32" s="7"/>
-      <c r="AQ32" s="7"/>
-      <c r="AR32" s="7"/>
-      <c r="AS32" s="7"/>
-      <c r="AT32" s="7"/>
-      <c r="AU32" s="7"/>
-      <c r="AV32" s="7"/>
-      <c r="AW32" s="8"/>
+      <c r="B32" s="6">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7">
+        <v>1</v>
+      </c>
+      <c r="I32" s="7">
+        <v>1</v>
+      </c>
+      <c r="J32" s="7">
+        <v>1</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="L32" s="7">
+        <v>1</v>
+      </c>
+      <c r="M32" s="7">
+        <v>1</v>
+      </c>
+      <c r="N32" s="7">
+        <v>1</v>
+      </c>
+      <c r="O32" s="7">
+        <v>1</v>
+      </c>
+      <c r="P32" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>0</v>
+      </c>
+      <c r="R32" s="7">
+        <v>0</v>
+      </c>
+      <c r="S32" s="7">
+        <v>0</v>
+      </c>
+      <c r="T32" s="7">
+        <v>0</v>
+      </c>
+      <c r="U32" s="7">
+        <v>0</v>
+      </c>
+      <c r="V32" s="7">
+        <v>0</v>
+      </c>
+      <c r="W32" s="7">
+        <v>0</v>
+      </c>
+      <c r="X32" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV32" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW32" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="7"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="7"/>
-      <c r="AE33" s="7"/>
-      <c r="AF33" s="7"/>
-      <c r="AG33" s="7"/>
-      <c r="AH33" s="7"/>
-      <c r="AI33" s="7"/>
-      <c r="AJ33" s="7"/>
-      <c r="AK33" s="7"/>
-      <c r="AL33" s="7"/>
-      <c r="AM33" s="7"/>
-      <c r="AN33" s="7"/>
-      <c r="AO33" s="7"/>
-      <c r="AP33" s="7"/>
-      <c r="AQ33" s="7"/>
-      <c r="AR33" s="7"/>
-      <c r="AS33" s="7"/>
-      <c r="AT33" s="7"/>
-      <c r="AU33" s="7"/>
-      <c r="AV33" s="7"/>
-      <c r="AW33" s="8"/>
+      <c r="B33" s="6">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7">
+        <v>1</v>
+      </c>
+      <c r="I33" s="7">
+        <v>1</v>
+      </c>
+      <c r="J33" s="7">
+        <v>1</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+      <c r="L33" s="7">
+        <v>1</v>
+      </c>
+      <c r="M33" s="7">
+        <v>1</v>
+      </c>
+      <c r="N33" s="7">
+        <v>1</v>
+      </c>
+      <c r="O33" s="7">
+        <v>1</v>
+      </c>
+      <c r="P33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>1</v>
+      </c>
+      <c r="R33" s="7">
+        <v>1</v>
+      </c>
+      <c r="S33" s="7">
+        <v>1</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7">
+        <v>1</v>
+      </c>
+      <c r="V33" s="7">
+        <v>1</v>
+      </c>
+      <c r="W33" s="7">
+        <v>1</v>
+      </c>
+      <c r="X33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AF33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AK33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AT33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV33" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW33" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="10"/>
-      <c r="W34" s="10"/>
-      <c r="X34" s="10"/>
-      <c r="Y34" s="10"/>
-      <c r="Z34" s="10"/>
-      <c r="AA34" s="10"/>
-      <c r="AB34" s="10"/>
-      <c r="AC34" s="10"/>
-      <c r="AD34" s="10"/>
-      <c r="AE34" s="10"/>
-      <c r="AF34" s="10"/>
-      <c r="AG34" s="10"/>
-      <c r="AH34" s="10"/>
-      <c r="AI34" s="10"/>
-      <c r="AJ34" s="10"/>
-      <c r="AK34" s="10"/>
-      <c r="AL34" s="10"/>
-      <c r="AM34" s="10"/>
-      <c r="AN34" s="10"/>
-      <c r="AO34" s="10"/>
-      <c r="AP34" s="10"/>
-      <c r="AQ34" s="10"/>
-      <c r="AR34" s="10"/>
-      <c r="AS34" s="10"/>
-      <c r="AT34" s="10"/>
-      <c r="AU34" s="10"/>
-      <c r="AV34" s="10"/>
-      <c r="AW34" s="11"/>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10">
+        <v>1</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
+      </c>
+      <c r="G34" s="10">
+        <v>1</v>
+      </c>
+      <c r="H34" s="10">
+        <v>1</v>
+      </c>
+      <c r="I34" s="10">
+        <v>1</v>
+      </c>
+      <c r="J34" s="10">
+        <v>1</v>
+      </c>
+      <c r="K34" s="10">
+        <v>1</v>
+      </c>
+      <c r="L34" s="10">
+        <v>1</v>
+      </c>
+      <c r="M34" s="10">
+        <v>1</v>
+      </c>
+      <c r="N34" s="10">
+        <v>1</v>
+      </c>
+      <c r="O34" s="10">
+        <v>1</v>
+      </c>
+      <c r="P34" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="10">
+        <v>0</v>
+      </c>
+      <c r="R34" s="10">
+        <v>0</v>
+      </c>
+      <c r="S34" s="10">
+        <v>0</v>
+      </c>
+      <c r="T34" s="10">
+        <v>0</v>
+      </c>
+      <c r="U34" s="10">
+        <v>0</v>
+      </c>
+      <c r="V34" s="10">
+        <v>0</v>
+      </c>
+      <c r="W34" s="10">
+        <v>0</v>
+      </c>
+      <c r="X34" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AL34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AN34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AO34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AP34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AR34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AT34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV34" s="10">
+        <v>1</v>
+      </c>
+      <c r="AW34" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
@@ -6048,6 +7462,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId3" name="ComboBox1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>49</xdr:col>
+                <xdr:colOff>466725</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>50</xdr:col>
+                <xdr:colOff>1295400</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId3" name="ComboBox1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Started new AA button
</commit_message>
<xml_diff>
--- a/RDS Agreement Manager.xlsx
+++ b/RDS Agreement Manager.xlsx
@@ -25,6 +25,7 @@
     <definedName name="Week2">Main!$B$12:$AW$18</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2841,6 +2842,10 @@
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3251,13 +3256,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>133349</xdr:colOff>
+          <xdr:colOff>133350</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>47624</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>57150</xdr:rowOff>
         </xdr:to>
@@ -3267,6 +3272,47 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>95250</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="BtnNewAA" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3581,7 +3627,7 @@
   <dimension ref="B2:AY98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,1027 +3641,355 @@
       <c r="I2" s="2"/>
     </row>
     <row r="4" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>1</v>
-      </c>
-      <c r="R4" s="4">
-        <v>1</v>
-      </c>
-      <c r="S4" s="4">
-        <v>1</v>
-      </c>
-      <c r="T4" s="4">
-        <v>1</v>
-      </c>
-      <c r="U4" s="4">
-        <v>1</v>
-      </c>
-      <c r="V4" s="4">
-        <v>1</v>
-      </c>
-      <c r="W4" s="4">
-        <v>1</v>
-      </c>
-      <c r="X4" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AP4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AR4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AS4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AT4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AU4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AV4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AW4" s="5">
-        <v>1</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="4"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="5"/>
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7">
-        <v>0</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0</v>
-      </c>
-      <c r="O5" s="7">
-        <v>0</v>
-      </c>
-      <c r="P5" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>1</v>
-      </c>
-      <c r="R5" s="7">
-        <v>1</v>
-      </c>
-      <c r="S5" s="7">
-        <v>1</v>
-      </c>
-      <c r="T5" s="7">
-        <v>1</v>
-      </c>
-      <c r="U5" s="7">
-        <v>1</v>
-      </c>
-      <c r="V5" s="7">
-        <v>1</v>
-      </c>
-      <c r="W5" s="7">
-        <v>1</v>
-      </c>
-      <c r="X5" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AU5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AV5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="8">
-        <v>1</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AN5" s="7"/>
+      <c r="AO5" s="7"/>
+      <c r="AP5" s="7"/>
+      <c r="AQ5" s="7"/>
+      <c r="AR5" s="7"/>
+      <c r="AS5" s="7"/>
+      <c r="AT5" s="7"/>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="7"/>
+      <c r="AW5" s="8"/>
     </row>
     <row r="6" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0</v>
-      </c>
-      <c r="L6" s="7">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0</v>
-      </c>
-      <c r="O6" s="7">
-        <v>0</v>
-      </c>
-      <c r="P6" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7">
-        <v>1</v>
-      </c>
-      <c r="S6" s="7">
-        <v>1</v>
-      </c>
-      <c r="T6" s="7">
-        <v>1</v>
-      </c>
-      <c r="U6" s="7">
-        <v>1</v>
-      </c>
-      <c r="V6" s="7">
-        <v>1</v>
-      </c>
-      <c r="W6" s="7">
-        <v>1</v>
-      </c>
-      <c r="X6" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AO6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AP6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AT6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AV6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW6" s="8">
-        <v>1</v>
-      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="7"/>
+      <c r="AQ6" s="7"/>
+      <c r="AR6" s="7"/>
+      <c r="AS6" s="7"/>
+      <c r="AT6" s="7"/>
+      <c r="AU6" s="7"/>
+      <c r="AV6" s="7"/>
+      <c r="AW6" s="8"/>
     </row>
     <row r="7" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0</v>
-      </c>
-      <c r="O7" s="7">
-        <v>0</v>
-      </c>
-      <c r="P7" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>1</v>
-      </c>
-      <c r="R7" s="7">
-        <v>1</v>
-      </c>
-      <c r="S7" s="7">
-        <v>1</v>
-      </c>
-      <c r="T7" s="7">
-        <v>1</v>
-      </c>
-      <c r="U7" s="7">
-        <v>1</v>
-      </c>
-      <c r="V7" s="7">
-        <v>1</v>
-      </c>
-      <c r="W7" s="7">
-        <v>1</v>
-      </c>
-      <c r="X7" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AM7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AN7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AO7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AP7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AT7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AU7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AV7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW7" s="8">
-        <v>1</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
+      <c r="AS7" s="7"/>
+      <c r="AT7" s="7"/>
+      <c r="AU7" s="7"/>
+      <c r="AV7" s="7"/>
+      <c r="AW7" s="8"/>
       <c r="AY7" s="2"/>
     </row>
     <row r="8" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7">
-        <v>1</v>
-      </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
-        <v>0</v>
-      </c>
-      <c r="L8" s="7">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
-        <v>0</v>
-      </c>
-      <c r="N8" s="7">
-        <v>0</v>
-      </c>
-      <c r="O8" s="7">
-        <v>0</v>
-      </c>
-      <c r="P8" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>1</v>
-      </c>
-      <c r="R8" s="7">
-        <v>1</v>
-      </c>
-      <c r="S8" s="7">
-        <v>1</v>
-      </c>
-      <c r="T8" s="7">
-        <v>1</v>
-      </c>
-      <c r="U8" s="7">
-        <v>1</v>
-      </c>
-      <c r="V8" s="7">
-        <v>1</v>
-      </c>
-      <c r="W8" s="7">
-        <v>1</v>
-      </c>
-      <c r="X8" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AM8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AN8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AO8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AP8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AT8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AU8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AV8" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW8" s="8">
-        <v>1</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="8"/>
     </row>
     <row r="9" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7">
-        <v>1</v>
-      </c>
-      <c r="K9" s="7">
-        <v>1</v>
-      </c>
-      <c r="L9" s="7">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7">
-        <v>1</v>
-      </c>
-      <c r="O9" s="7">
-        <v>1</v>
-      </c>
-      <c r="P9" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>1</v>
-      </c>
-      <c r="R9" s="7">
-        <v>1</v>
-      </c>
-      <c r="S9" s="7">
-        <v>1</v>
-      </c>
-      <c r="T9" s="7">
-        <v>1</v>
-      </c>
-      <c r="U9" s="7">
-        <v>1</v>
-      </c>
-      <c r="V9" s="7">
-        <v>1</v>
-      </c>
-      <c r="W9" s="7">
-        <v>1</v>
-      </c>
-      <c r="X9" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AV9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="8">
-        <v>0</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+      <c r="AM9" s="7"/>
+      <c r="AN9" s="7"/>
+      <c r="AO9" s="7"/>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="7"/>
+      <c r="AT9" s="7"/>
+      <c r="AU9" s="7"/>
+      <c r="AV9" s="7"/>
+      <c r="AW9" s="8"/>
     </row>
     <row r="10" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10">
-        <v>0</v>
-      </c>
-      <c r="J10" s="10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="10">
-        <v>0</v>
-      </c>
-      <c r="O10" s="10">
-        <v>0</v>
-      </c>
-      <c r="P10" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>0</v>
-      </c>
-      <c r="R10" s="10">
-        <v>0</v>
-      </c>
-      <c r="S10" s="10">
-        <v>0</v>
-      </c>
-      <c r="T10" s="10">
-        <v>1</v>
-      </c>
-      <c r="U10" s="10">
-        <v>1</v>
-      </c>
-      <c r="V10" s="10">
-        <v>1</v>
-      </c>
-      <c r="W10" s="10">
-        <v>1</v>
-      </c>
-      <c r="X10" s="10">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="10">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AJ10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AK10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AM10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AN10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AO10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AP10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AQ10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AR10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AT10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AU10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AV10" s="10">
-        <v>1</v>
-      </c>
-      <c r="AW10" s="11">
-        <v>1</v>
-      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="10"/>
+      <c r="AO10" s="10"/>
+      <c r="AP10" s="10"/>
+      <c r="AQ10" s="10"/>
+      <c r="AR10" s="10"/>
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
+      <c r="AW10" s="11"/>
     </row>
     <row r="11" spans="2:51" x14ac:dyDescent="0.25">
       <c r="AY11" s="2"/>
@@ -8580,7 +7954,7 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1030" r:id="rId12" name="TxtTemplateDate">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>50</xdr:col>
@@ -8604,8 +7978,8 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId14" name="TxtNoWeeks">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+        <control shapeId="1029" r:id="rId13" name="TxtNoWeeks">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8624,13 +7998,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId14" name="TxtNoWeeks"/>
+        <control shapeId="1029" r:id="rId13" name="TxtNoWeeks"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId16" name="TxtName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="1028" r:id="rId15" name="TxtName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8649,13 +8023,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId16" name="TxtName"/>
+        <control shapeId="1028" r:id="rId15" name="TxtName"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId18" name="TxtCrewNo">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+        <control shapeId="1027" r:id="rId16" name="TxtCrewNo">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8674,13 +8048,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId18" name="TxtCrewNo"/>
+        <control shapeId="1027" r:id="rId16" name="TxtCrewNo"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId20" name="CmoStation1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+        <control shapeId="1025" r:id="rId17" name="CmoStation1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8699,13 +8073,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId20" name="CmoStation1"/>
+        <control shapeId="1025" r:id="rId17" name="CmoStation1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId22" name="CmoStation2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
+        <control shapeId="1026" r:id="rId19" name="CmoStation2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8724,7 +8098,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId22" name="CmoStation2"/>
+        <control shapeId="1026" r:id="rId19" name="CmoStation2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId21" name="BtnNewAA">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId21" name="BtnNewAA"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Format range Update AA
</commit_message>
<xml_diff>
--- a/RDS Agreement Manager.xlsx
+++ b/RDS Agreement Manager.xlsx
@@ -2709,12 +2709,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF322924"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -2809,19 +2815,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2845,15 +2872,19 @@
 </file>
 
 <file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2861,7 +2892,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2877,7 +2908,7 @@
 </file>
 
 <file path=xl/activeX/activeX9.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3333,6 +3364,47 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>21</xdr:col>
+          <xdr:colOff>95250</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>29</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="BtnUpdateAA" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -3627,7 +3699,7 @@
   <dimension ref="B2:AY98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3641,708 +3713,2052 @@
       <c r="I2" s="2"/>
     </row>
     <row r="4" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4"/>
-      <c r="AW4" s="5"/>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="4">
+        <v>0</v>
+      </c>
+      <c r="X4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="7"/>
-      <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AP5" s="7"/>
-      <c r="AQ5" s="7"/>
-      <c r="AR5" s="7"/>
-      <c r="AS5" s="7"/>
-      <c r="AT5" s="7"/>
-      <c r="AU5" s="7"/>
-      <c r="AV5" s="7"/>
-      <c r="AW5" s="8"/>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>0</v>
+      </c>
+      <c r="R5" s="7">
+        <v>0</v>
+      </c>
+      <c r="S5" s="7">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7">
+        <v>0</v>
+      </c>
+      <c r="U5" s="7">
+        <v>0</v>
+      </c>
+      <c r="V5" s="7">
+        <v>0</v>
+      </c>
+      <c r="W5" s="7">
+        <v>0</v>
+      </c>
+      <c r="X5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7"/>
-      <c r="AG6" s="7"/>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="7"/>
-      <c r="AJ6" s="7"/>
-      <c r="AK6" s="7"/>
-      <c r="AL6" s="7"/>
-      <c r="AM6" s="7"/>
-      <c r="AN6" s="7"/>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="7"/>
-      <c r="AQ6" s="7"/>
-      <c r="AR6" s="7"/>
-      <c r="AS6" s="7"/>
-      <c r="AT6" s="7"/>
-      <c r="AU6" s="7"/>
-      <c r="AV6" s="7"/>
-      <c r="AW6" s="8"/>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>0</v>
+      </c>
+      <c r="R6" s="7">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7">
+        <v>0</v>
+      </c>
+      <c r="V6" s="7">
+        <v>0</v>
+      </c>
+      <c r="W6" s="7">
+        <v>0</v>
+      </c>
+      <c r="X6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
-      <c r="AE7" s="7"/>
-      <c r="AF7" s="7"/>
-      <c r="AG7" s="7"/>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="7"/>
-      <c r="AJ7" s="7"/>
-      <c r="AK7" s="7"/>
-      <c r="AL7" s="7"/>
-      <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-      <c r="AR7" s="7"/>
-      <c r="AS7" s="7"/>
-      <c r="AT7" s="7"/>
-      <c r="AU7" s="7"/>
-      <c r="AV7" s="7"/>
-      <c r="AW7" s="8"/>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>0</v>
+      </c>
+      <c r="R7" s="7">
+        <v>0</v>
+      </c>
+      <c r="S7" s="7">
+        <v>0</v>
+      </c>
+      <c r="T7" s="7">
+        <v>0</v>
+      </c>
+      <c r="U7" s="7">
+        <v>0</v>
+      </c>
+      <c r="V7" s="7">
+        <v>0</v>
+      </c>
+      <c r="W7" s="7">
+        <v>0</v>
+      </c>
+      <c r="X7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="8">
+        <v>0</v>
+      </c>
       <c r="AY7" s="2"/>
     </row>
     <row r="8" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="7"/>
-      <c r="AG8" s="7"/>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="7"/>
-      <c r="AJ8" s="7"/>
-      <c r="AK8" s="7"/>
-      <c r="AL8" s="7"/>
-      <c r="AM8" s="7"/>
-      <c r="AN8" s="7"/>
-      <c r="AO8" s="7"/>
-      <c r="AP8" s="7"/>
-      <c r="AQ8" s="7"/>
-      <c r="AR8" s="7"/>
-      <c r="AS8" s="7"/>
-      <c r="AT8" s="7"/>
-      <c r="AU8" s="7"/>
-      <c r="AV8" s="7"/>
-      <c r="AW8" s="8"/>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>0</v>
+      </c>
+      <c r="R8" s="7">
+        <v>0</v>
+      </c>
+      <c r="S8" s="7">
+        <v>0</v>
+      </c>
+      <c r="T8" s="7">
+        <v>0</v>
+      </c>
+      <c r="U8" s="7">
+        <v>0</v>
+      </c>
+      <c r="V8" s="7">
+        <v>0</v>
+      </c>
+      <c r="W8" s="7">
+        <v>0</v>
+      </c>
+      <c r="X8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
-      <c r="AE9" s="7"/>
-      <c r="AF9" s="7"/>
-      <c r="AG9" s="7"/>
-      <c r="AH9" s="7"/>
-      <c r="AI9" s="7"/>
-      <c r="AJ9" s="7"/>
-      <c r="AK9" s="7"/>
-      <c r="AL9" s="7"/>
-      <c r="AM9" s="7"/>
-      <c r="AN9" s="7"/>
-      <c r="AO9" s="7"/>
-      <c r="AP9" s="7"/>
-      <c r="AQ9" s="7"/>
-      <c r="AR9" s="7"/>
-      <c r="AS9" s="7"/>
-      <c r="AT9" s="7"/>
-      <c r="AU9" s="7"/>
-      <c r="AV9" s="7"/>
-      <c r="AW9" s="8"/>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7">
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>0</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0</v>
+      </c>
+      <c r="S9" s="7">
+        <v>0</v>
+      </c>
+      <c r="T9" s="7">
+        <v>0</v>
+      </c>
+      <c r="U9" s="7">
+        <v>0</v>
+      </c>
+      <c r="V9" s="7">
+        <v>0</v>
+      </c>
+      <c r="W9" s="7">
+        <v>0</v>
+      </c>
+      <c r="X9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="10"/>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="10"/>
-      <c r="AL10" s="10"/>
-      <c r="AM10" s="10"/>
-      <c r="AN10" s="10"/>
-      <c r="AO10" s="10"/>
-      <c r="AP10" s="10"/>
-      <c r="AQ10" s="10"/>
-      <c r="AR10" s="10"/>
-      <c r="AS10" s="10"/>
-      <c r="AT10" s="10"/>
-      <c r="AU10" s="10"/>
-      <c r="AV10" s="10"/>
-      <c r="AW10" s="11"/>
+      <c r="B10" s="9">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>0</v>
+      </c>
+      <c r="R10" s="10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="10">
+        <v>0</v>
+      </c>
+      <c r="U10" s="10">
+        <v>0</v>
+      </c>
+      <c r="V10" s="10">
+        <v>0</v>
+      </c>
+      <c r="W10" s="10">
+        <v>0</v>
+      </c>
+      <c r="X10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:51" x14ac:dyDescent="0.25">
       <c r="AY11" s="2"/>
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
-      <c r="AG12" s="4"/>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="4"/>
-      <c r="AJ12" s="4"/>
-      <c r="AK12" s="4"/>
-      <c r="AL12" s="4"/>
-      <c r="AM12" s="4"/>
-      <c r="AN12" s="4"/>
-      <c r="AO12" s="4"/>
-      <c r="AP12" s="4"/>
-      <c r="AQ12" s="4"/>
-      <c r="AR12" s="4"/>
-      <c r="AS12" s="4"/>
-      <c r="AT12" s="4"/>
-      <c r="AU12" s="4"/>
-      <c r="AV12" s="4"/>
-      <c r="AW12" s="5"/>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
+        <v>0</v>
+      </c>
+      <c r="V12" s="4">
+        <v>0</v>
+      </c>
+      <c r="W12" s="4">
+        <v>0</v>
+      </c>
+      <c r="X12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="7"/>
-      <c r="AE13" s="7"/>
-      <c r="AF13" s="7"/>
-      <c r="AG13" s="7"/>
-      <c r="AH13" s="7"/>
-      <c r="AI13" s="7"/>
-      <c r="AJ13" s="7"/>
-      <c r="AK13" s="7"/>
-      <c r="AL13" s="7"/>
-      <c r="AM13" s="7"/>
-      <c r="AN13" s="7"/>
-      <c r="AO13" s="7"/>
-      <c r="AP13" s="7"/>
-      <c r="AQ13" s="7"/>
-      <c r="AR13" s="7"/>
-      <c r="AS13" s="7"/>
-      <c r="AT13" s="7"/>
-      <c r="AU13" s="7"/>
-      <c r="AV13" s="7"/>
-      <c r="AW13" s="8"/>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
+        <v>0</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>0</v>
+      </c>
+      <c r="R13" s="7">
+        <v>0</v>
+      </c>
+      <c r="S13" s="7">
+        <v>0</v>
+      </c>
+      <c r="T13" s="7">
+        <v>0</v>
+      </c>
+      <c r="U13" s="7">
+        <v>0</v>
+      </c>
+      <c r="V13" s="7">
+        <v>0</v>
+      </c>
+      <c r="W13" s="7">
+        <v>0</v>
+      </c>
+      <c r="X13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
-      <c r="AE14" s="7"/>
-      <c r="AF14" s="7"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="7"/>
-      <c r="AK14" s="7"/>
-      <c r="AL14" s="7"/>
-      <c r="AM14" s="7"/>
-      <c r="AN14" s="7"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="7"/>
-      <c r="AQ14" s="7"/>
-      <c r="AR14" s="7"/>
-      <c r="AS14" s="7"/>
-      <c r="AT14" s="7"/>
-      <c r="AU14" s="7"/>
-      <c r="AV14" s="7"/>
-      <c r="AW14" s="8"/>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7">
+        <v>0</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>0</v>
+      </c>
+      <c r="R14" s="7">
+        <v>0</v>
+      </c>
+      <c r="S14" s="7">
+        <v>0</v>
+      </c>
+      <c r="T14" s="7">
+        <v>0</v>
+      </c>
+      <c r="U14" s="7">
+        <v>0</v>
+      </c>
+      <c r="V14" s="7">
+        <v>0</v>
+      </c>
+      <c r="W14" s="7">
+        <v>0</v>
+      </c>
+      <c r="X14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="7"/>
-      <c r="AI15" s="7"/>
-      <c r="AJ15" s="7"/>
-      <c r="AK15" s="7"/>
-      <c r="AL15" s="7"/>
-      <c r="AM15" s="7"/>
-      <c r="AN15" s="7"/>
-      <c r="AO15" s="7"/>
-      <c r="AP15" s="7"/>
-      <c r="AQ15" s="7"/>
-      <c r="AR15" s="7"/>
-      <c r="AS15" s="7"/>
-      <c r="AT15" s="7"/>
-      <c r="AU15" s="7"/>
-      <c r="AV15" s="7"/>
-      <c r="AW15" s="8"/>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>0</v>
+      </c>
+      <c r="R15" s="7">
+        <v>0</v>
+      </c>
+      <c r="S15" s="7">
+        <v>0</v>
+      </c>
+      <c r="T15" s="7">
+        <v>0</v>
+      </c>
+      <c r="U15" s="7">
+        <v>0</v>
+      </c>
+      <c r="V15" s="7">
+        <v>0</v>
+      </c>
+      <c r="W15" s="7">
+        <v>0</v>
+      </c>
+      <c r="X15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV15" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:51" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="7"/>
-      <c r="AE16" s="7"/>
-      <c r="AF16" s="7"/>
-      <c r="AG16" s="7"/>
-      <c r="AH16" s="7"/>
-      <c r="AI16" s="7"/>
-      <c r="AJ16" s="7"/>
-      <c r="AK16" s="7"/>
-      <c r="AL16" s="7"/>
-      <c r="AM16" s="7"/>
-      <c r="AN16" s="7"/>
-      <c r="AO16" s="7"/>
-      <c r="AP16" s="7"/>
-      <c r="AQ16" s="7"/>
-      <c r="AR16" s="7"/>
-      <c r="AS16" s="7"/>
-      <c r="AT16" s="7"/>
-      <c r="AU16" s="7"/>
-      <c r="AV16" s="7"/>
-      <c r="AW16" s="8"/>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7">
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0</v>
+      </c>
+      <c r="O16" s="7">
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>0</v>
+      </c>
+      <c r="R16" s="7">
+        <v>0</v>
+      </c>
+      <c r="S16" s="7">
+        <v>0</v>
+      </c>
+      <c r="T16" s="7">
+        <v>0</v>
+      </c>
+      <c r="U16" s="7">
+        <v>0</v>
+      </c>
+      <c r="V16" s="7">
+        <v>0</v>
+      </c>
+      <c r="W16" s="7">
+        <v>0</v>
+      </c>
+      <c r="X16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
-      <c r="AF17" s="7"/>
-      <c r="AG17" s="7"/>
-      <c r="AH17" s="7"/>
-      <c r="AI17" s="7"/>
-      <c r="AJ17" s="7"/>
-      <c r="AK17" s="7"/>
-      <c r="AL17" s="7"/>
-      <c r="AM17" s="7"/>
-      <c r="AN17" s="7"/>
-      <c r="AO17" s="7"/>
-      <c r="AP17" s="7"/>
-      <c r="AQ17" s="7"/>
-      <c r="AR17" s="7"/>
-      <c r="AS17" s="7"/>
-      <c r="AT17" s="7"/>
-      <c r="AU17" s="7"/>
-      <c r="AV17" s="7"/>
-      <c r="AW17" s="8"/>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+      <c r="O17" s="7">
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>0</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0</v>
+      </c>
+      <c r="S17" s="7">
+        <v>0</v>
+      </c>
+      <c r="T17" s="7">
+        <v>0</v>
+      </c>
+      <c r="U17" s="7">
+        <v>0</v>
+      </c>
+      <c r="V17" s="7">
+        <v>0</v>
+      </c>
+      <c r="W17" s="7">
+        <v>0</v>
+      </c>
+      <c r="X17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW17" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="10"/>
-      <c r="AJ18" s="10"/>
-      <c r="AK18" s="10"/>
-      <c r="AL18" s="10"/>
-      <c r="AM18" s="10"/>
-      <c r="AN18" s="10"/>
-      <c r="AO18" s="10"/>
-      <c r="AP18" s="10"/>
-      <c r="AQ18" s="10"/>
-      <c r="AR18" s="10"/>
-      <c r="AS18" s="10"/>
-      <c r="AT18" s="10"/>
-      <c r="AU18" s="10"/>
-      <c r="AV18" s="10"/>
-      <c r="AW18" s="11"/>
+      <c r="B18" s="9">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0</v>
+      </c>
+      <c r="M18" s="10">
+        <v>0</v>
+      </c>
+      <c r="N18" s="10">
+        <v>0</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0</v>
+      </c>
+      <c r="P18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>0</v>
+      </c>
+      <c r="R18" s="10">
+        <v>0</v>
+      </c>
+      <c r="S18" s="10">
+        <v>0</v>
+      </c>
+      <c r="T18" s="10">
+        <v>0</v>
+      </c>
+      <c r="U18" s="10">
+        <v>0</v>
+      </c>
+      <c r="V18" s="10">
+        <v>0</v>
+      </c>
+      <c r="W18" s="10">
+        <v>0</v>
+      </c>
+      <c r="X18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -7495,354 +8911,354 @@
       <c r="AW90" s="11"/>
     </row>
     <row r="92" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
-      <c r="K92" s="4"/>
-      <c r="L92" s="4"/>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
-      <c r="Q92" s="4"/>
-      <c r="R92" s="4"/>
-      <c r="S92" s="4"/>
-      <c r="T92" s="4"/>
-      <c r="U92" s="4"/>
-      <c r="V92" s="4"/>
-      <c r="W92" s="4"/>
-      <c r="X92" s="4"/>
-      <c r="Y92" s="4"/>
-      <c r="Z92" s="4"/>
-      <c r="AA92" s="4"/>
-      <c r="AB92" s="4"/>
-      <c r="AC92" s="4"/>
-      <c r="AD92" s="4"/>
-      <c r="AE92" s="4"/>
-      <c r="AF92" s="4"/>
-      <c r="AG92" s="4"/>
-      <c r="AH92" s="4"/>
-      <c r="AI92" s="4"/>
-      <c r="AJ92" s="4"/>
-      <c r="AK92" s="4"/>
-      <c r="AL92" s="4"/>
-      <c r="AM92" s="4"/>
-      <c r="AN92" s="4"/>
-      <c r="AO92" s="4"/>
-      <c r="AP92" s="4"/>
-      <c r="AQ92" s="4"/>
-      <c r="AR92" s="4"/>
-      <c r="AS92" s="4"/>
-      <c r="AT92" s="4"/>
-      <c r="AU92" s="4"/>
-      <c r="AV92" s="4"/>
-      <c r="AW92" s="5"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
+      <c r="J92" s="12"/>
+      <c r="K92" s="12"/>
+      <c r="L92" s="12"/>
+      <c r="M92" s="12"/>
+      <c r="N92" s="12"/>
+      <c r="O92" s="12"/>
+      <c r="P92" s="12"/>
+      <c r="Q92" s="12"/>
+      <c r="R92" s="12"/>
+      <c r="S92" s="12"/>
+      <c r="T92" s="12"/>
+      <c r="U92" s="12"/>
+      <c r="V92" s="12"/>
+      <c r="W92" s="12"/>
+      <c r="X92" s="12"/>
+      <c r="Y92" s="12"/>
+      <c r="Z92" s="12"/>
+      <c r="AA92" s="12"/>
+      <c r="AB92" s="12"/>
+      <c r="AC92" s="12"/>
+      <c r="AD92" s="12"/>
+      <c r="AE92" s="12"/>
+      <c r="AF92" s="12"/>
+      <c r="AG92" s="12"/>
+      <c r="AH92" s="12"/>
+      <c r="AI92" s="12"/>
+      <c r="AJ92" s="12"/>
+      <c r="AK92" s="12"/>
+      <c r="AL92" s="12"/>
+      <c r="AM92" s="12"/>
+      <c r="AN92" s="12"/>
+      <c r="AO92" s="12"/>
+      <c r="AP92" s="12"/>
+      <c r="AQ92" s="12"/>
+      <c r="AR92" s="12"/>
+      <c r="AS92" s="12"/>
+      <c r="AT92" s="12"/>
+      <c r="AU92" s="12"/>
+      <c r="AV92" s="12"/>
+      <c r="AW92" s="12"/>
     </row>
     <row r="93" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B93" s="6"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="7"/>
-      <c r="J93" s="7"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="7"/>
-      <c r="M93" s="7"/>
-      <c r="N93" s="7"/>
-      <c r="O93" s="7"/>
-      <c r="P93" s="7"/>
-      <c r="Q93" s="7"/>
-      <c r="R93" s="7"/>
-      <c r="S93" s="7"/>
-      <c r="T93" s="7"/>
-      <c r="U93" s="7"/>
-      <c r="V93" s="7"/>
-      <c r="W93" s="7"/>
-      <c r="X93" s="7"/>
-      <c r="Y93" s="7"/>
-      <c r="Z93" s="7"/>
-      <c r="AA93" s="7"/>
-      <c r="AB93" s="7"/>
-      <c r="AC93" s="7"/>
-      <c r="AD93" s="7"/>
-      <c r="AE93" s="7"/>
-      <c r="AF93" s="7"/>
-      <c r="AG93" s="7"/>
-      <c r="AH93" s="7"/>
-      <c r="AI93" s="7"/>
-      <c r="AJ93" s="7"/>
-      <c r="AK93" s="7"/>
-      <c r="AL93" s="7"/>
-      <c r="AM93" s="7"/>
-      <c r="AN93" s="7"/>
-      <c r="AO93" s="7"/>
-      <c r="AP93" s="7"/>
-      <c r="AQ93" s="7"/>
-      <c r="AR93" s="7"/>
-      <c r="AS93" s="7"/>
-      <c r="AT93" s="7"/>
-      <c r="AU93" s="7"/>
-      <c r="AV93" s="7"/>
-      <c r="AW93" s="8"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
+      <c r="L93" s="12"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="12"/>
+      <c r="P93" s="12"/>
+      <c r="Q93" s="12"/>
+      <c r="R93" s="12"/>
+      <c r="S93" s="12"/>
+      <c r="T93" s="12"/>
+      <c r="U93" s="12"/>
+      <c r="V93" s="12"/>
+      <c r="W93" s="12"/>
+      <c r="X93" s="12"/>
+      <c r="Y93" s="12"/>
+      <c r="Z93" s="12"/>
+      <c r="AA93" s="12"/>
+      <c r="AB93" s="12"/>
+      <c r="AC93" s="12"/>
+      <c r="AD93" s="12"/>
+      <c r="AE93" s="12"/>
+      <c r="AF93" s="12"/>
+      <c r="AG93" s="12"/>
+      <c r="AH93" s="12"/>
+      <c r="AI93" s="12"/>
+      <c r="AJ93" s="12"/>
+      <c r="AK93" s="12"/>
+      <c r="AL93" s="12"/>
+      <c r="AM93" s="12"/>
+      <c r="AN93" s="12"/>
+      <c r="AO93" s="12"/>
+      <c r="AP93" s="12"/>
+      <c r="AQ93" s="12"/>
+      <c r="AR93" s="12"/>
+      <c r="AS93" s="12"/>
+      <c r="AT93" s="12"/>
+      <c r="AU93" s="12"/>
+      <c r="AV93" s="12"/>
+      <c r="AW93" s="12"/>
     </row>
     <row r="94" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B94" s="6"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
-      <c r="M94" s="7"/>
-      <c r="N94" s="7"/>
-      <c r="O94" s="7"/>
-      <c r="P94" s="7"/>
-      <c r="Q94" s="7"/>
-      <c r="R94" s="7"/>
-      <c r="S94" s="7"/>
-      <c r="T94" s="7"/>
-      <c r="U94" s="7"/>
-      <c r="V94" s="7"/>
-      <c r="W94" s="7"/>
-      <c r="X94" s="7"/>
-      <c r="Y94" s="7"/>
-      <c r="Z94" s="7"/>
-      <c r="AA94" s="7"/>
-      <c r="AB94" s="7"/>
-      <c r="AC94" s="7"/>
-      <c r="AD94" s="7"/>
-      <c r="AE94" s="7"/>
-      <c r="AF94" s="7"/>
-      <c r="AG94" s="7"/>
-      <c r="AH94" s="7"/>
-      <c r="AI94" s="7"/>
-      <c r="AJ94" s="7"/>
-      <c r="AK94" s="7"/>
-      <c r="AL94" s="7"/>
-      <c r="AM94" s="7"/>
-      <c r="AN94" s="7"/>
-      <c r="AO94" s="7"/>
-      <c r="AP94" s="7"/>
-      <c r="AQ94" s="7"/>
-      <c r="AR94" s="7"/>
-      <c r="AS94" s="7"/>
-      <c r="AT94" s="7"/>
-      <c r="AU94" s="7"/>
-      <c r="AV94" s="7"/>
-      <c r="AW94" s="8"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
+      <c r="J94" s="12"/>
+      <c r="K94" s="12"/>
+      <c r="L94" s="12"/>
+      <c r="M94" s="12"/>
+      <c r="N94" s="12"/>
+      <c r="O94" s="12"/>
+      <c r="P94" s="12"/>
+      <c r="Q94" s="12"/>
+      <c r="R94" s="12"/>
+      <c r="S94" s="12"/>
+      <c r="T94" s="12"/>
+      <c r="U94" s="12"/>
+      <c r="V94" s="12"/>
+      <c r="W94" s="12"/>
+      <c r="X94" s="12"/>
+      <c r="Y94" s="12"/>
+      <c r="Z94" s="12"/>
+      <c r="AA94" s="12"/>
+      <c r="AB94" s="12"/>
+      <c r="AC94" s="12"/>
+      <c r="AD94" s="12"/>
+      <c r="AE94" s="12"/>
+      <c r="AF94" s="12"/>
+      <c r="AG94" s="12"/>
+      <c r="AH94" s="12"/>
+      <c r="AI94" s="12"/>
+      <c r="AJ94" s="12"/>
+      <c r="AK94" s="12"/>
+      <c r="AL94" s="12"/>
+      <c r="AM94" s="12"/>
+      <c r="AN94" s="12"/>
+      <c r="AO94" s="12"/>
+      <c r="AP94" s="12"/>
+      <c r="AQ94" s="12"/>
+      <c r="AR94" s="12"/>
+      <c r="AS94" s="12"/>
+      <c r="AT94" s="12"/>
+      <c r="AU94" s="12"/>
+      <c r="AV94" s="12"/>
+      <c r="AW94" s="12"/>
     </row>
     <row r="95" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B95" s="6"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="7"/>
-      <c r="I95" s="7"/>
-      <c r="J95" s="7"/>
-      <c r="K95" s="7"/>
-      <c r="L95" s="7"/>
-      <c r="M95" s="7"/>
-      <c r="N95" s="7"/>
-      <c r="O95" s="7"/>
-      <c r="P95" s="7"/>
-      <c r="Q95" s="7"/>
-      <c r="R95" s="7"/>
-      <c r="S95" s="7"/>
-      <c r="T95" s="7"/>
-      <c r="U95" s="7"/>
-      <c r="V95" s="7"/>
-      <c r="W95" s="7"/>
-      <c r="X95" s="7"/>
-      <c r="Y95" s="7"/>
-      <c r="Z95" s="7"/>
-      <c r="AA95" s="7"/>
-      <c r="AB95" s="7"/>
-      <c r="AC95" s="7"/>
-      <c r="AD95" s="7"/>
-      <c r="AE95" s="7"/>
-      <c r="AF95" s="7"/>
-      <c r="AG95" s="7"/>
-      <c r="AH95" s="7"/>
-      <c r="AI95" s="7"/>
-      <c r="AJ95" s="7"/>
-      <c r="AK95" s="7"/>
-      <c r="AL95" s="7"/>
-      <c r="AM95" s="7"/>
-      <c r="AN95" s="7"/>
-      <c r="AO95" s="7"/>
-      <c r="AP95" s="7"/>
-      <c r="AQ95" s="7"/>
-      <c r="AR95" s="7"/>
-      <c r="AS95" s="7"/>
-      <c r="AT95" s="7"/>
-      <c r="AU95" s="7"/>
-      <c r="AV95" s="7"/>
-      <c r="AW95" s="8"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
+      <c r="M95" s="12"/>
+      <c r="N95" s="12"/>
+      <c r="O95" s="12"/>
+      <c r="P95" s="12"/>
+      <c r="Q95" s="12"/>
+      <c r="R95" s="12"/>
+      <c r="S95" s="12"/>
+      <c r="T95" s="12"/>
+      <c r="U95" s="12"/>
+      <c r="V95" s="12"/>
+      <c r="W95" s="12"/>
+      <c r="X95" s="12"/>
+      <c r="Y95" s="12"/>
+      <c r="Z95" s="12"/>
+      <c r="AA95" s="12"/>
+      <c r="AB95" s="12"/>
+      <c r="AC95" s="12"/>
+      <c r="AD95" s="12"/>
+      <c r="AE95" s="12"/>
+      <c r="AF95" s="12"/>
+      <c r="AG95" s="12"/>
+      <c r="AH95" s="12"/>
+      <c r="AI95" s="12"/>
+      <c r="AJ95" s="12"/>
+      <c r="AK95" s="12"/>
+      <c r="AL95" s="12"/>
+      <c r="AM95" s="12"/>
+      <c r="AN95" s="12"/>
+      <c r="AO95" s="12"/>
+      <c r="AP95" s="12"/>
+      <c r="AQ95" s="12"/>
+      <c r="AR95" s="12"/>
+      <c r="AS95" s="12"/>
+      <c r="AT95" s="12"/>
+      <c r="AU95" s="12"/>
+      <c r="AV95" s="12"/>
+      <c r="AW95" s="12"/>
     </row>
     <row r="96" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B96" s="6"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
-      <c r="I96" s="7"/>
-      <c r="J96" s="7"/>
-      <c r="K96" s="7"/>
-      <c r="L96" s="7"/>
-      <c r="M96" s="7"/>
-      <c r="N96" s="7"/>
-      <c r="O96" s="7"/>
-      <c r="P96" s="7"/>
-      <c r="Q96" s="7"/>
-      <c r="R96" s="7"/>
-      <c r="S96" s="7"/>
-      <c r="T96" s="7"/>
-      <c r="U96" s="7"/>
-      <c r="V96" s="7"/>
-      <c r="W96" s="7"/>
-      <c r="X96" s="7"/>
-      <c r="Y96" s="7"/>
-      <c r="Z96" s="7"/>
-      <c r="AA96" s="7"/>
-      <c r="AB96" s="7"/>
-      <c r="AC96" s="7"/>
-      <c r="AD96" s="7"/>
-      <c r="AE96" s="7"/>
-      <c r="AF96" s="7"/>
-      <c r="AG96" s="7"/>
-      <c r="AH96" s="7"/>
-      <c r="AI96" s="7"/>
-      <c r="AJ96" s="7"/>
-      <c r="AK96" s="7"/>
-      <c r="AL96" s="7"/>
-      <c r="AM96" s="7"/>
-      <c r="AN96" s="7"/>
-      <c r="AO96" s="7"/>
-      <c r="AP96" s="7"/>
-      <c r="AQ96" s="7"/>
-      <c r="AR96" s="7"/>
-      <c r="AS96" s="7"/>
-      <c r="AT96" s="7"/>
-      <c r="AU96" s="7"/>
-      <c r="AV96" s="7"/>
-      <c r="AW96" s="8"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="12"/>
+      <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
+      <c r="L96" s="12"/>
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+      <c r="O96" s="12"/>
+      <c r="P96" s="12"/>
+      <c r="Q96" s="12"/>
+      <c r="R96" s="12"/>
+      <c r="S96" s="12"/>
+      <c r="T96" s="12"/>
+      <c r="U96" s="12"/>
+      <c r="V96" s="12"/>
+      <c r="W96" s="12"/>
+      <c r="X96" s="12"/>
+      <c r="Y96" s="12"/>
+      <c r="Z96" s="12"/>
+      <c r="AA96" s="12"/>
+      <c r="AB96" s="12"/>
+      <c r="AC96" s="12"/>
+      <c r="AD96" s="12"/>
+      <c r="AE96" s="12"/>
+      <c r="AF96" s="12"/>
+      <c r="AG96" s="12"/>
+      <c r="AH96" s="12"/>
+      <c r="AI96" s="12"/>
+      <c r="AJ96" s="12"/>
+      <c r="AK96" s="12"/>
+      <c r="AL96" s="12"/>
+      <c r="AM96" s="12"/>
+      <c r="AN96" s="12"/>
+      <c r="AO96" s="12"/>
+      <c r="AP96" s="12"/>
+      <c r="AQ96" s="12"/>
+      <c r="AR96" s="12"/>
+      <c r="AS96" s="12"/>
+      <c r="AT96" s="12"/>
+      <c r="AU96" s="12"/>
+      <c r="AV96" s="12"/>
+      <c r="AW96" s="12"/>
     </row>
     <row r="97" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B97" s="6"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7"/>
-      <c r="H97" s="7"/>
-      <c r="I97" s="7"/>
-      <c r="J97" s="7"/>
-      <c r="K97" s="7"/>
-      <c r="L97" s="7"/>
-      <c r="M97" s="7"/>
-      <c r="N97" s="7"/>
-      <c r="O97" s="7"/>
-      <c r="P97" s="7"/>
-      <c r="Q97" s="7"/>
-      <c r="R97" s="7"/>
-      <c r="S97" s="7"/>
-      <c r="T97" s="7"/>
-      <c r="U97" s="7"/>
-      <c r="V97" s="7"/>
-      <c r="W97" s="7"/>
-      <c r="X97" s="7"/>
-      <c r="Y97" s="7"/>
-      <c r="Z97" s="7"/>
-      <c r="AA97" s="7"/>
-      <c r="AB97" s="7"/>
-      <c r="AC97" s="7"/>
-      <c r="AD97" s="7"/>
-      <c r="AE97" s="7"/>
-      <c r="AF97" s="7"/>
-      <c r="AG97" s="7"/>
-      <c r="AH97" s="7"/>
-      <c r="AI97" s="7"/>
-      <c r="AJ97" s="7"/>
-      <c r="AK97" s="7"/>
-      <c r="AL97" s="7"/>
-      <c r="AM97" s="7"/>
-      <c r="AN97" s="7"/>
-      <c r="AO97" s="7"/>
-      <c r="AP97" s="7"/>
-      <c r="AQ97" s="7"/>
-      <c r="AR97" s="7"/>
-      <c r="AS97" s="7"/>
-      <c r="AT97" s="7"/>
-      <c r="AU97" s="7"/>
-      <c r="AV97" s="7"/>
-      <c r="AW97" s="8"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="12"/>
+      <c r="P97" s="12"/>
+      <c r="Q97" s="12"/>
+      <c r="R97" s="12"/>
+      <c r="S97" s="12"/>
+      <c r="T97" s="12"/>
+      <c r="U97" s="12"/>
+      <c r="V97" s="12"/>
+      <c r="W97" s="12"/>
+      <c r="X97" s="12"/>
+      <c r="Y97" s="12"/>
+      <c r="Z97" s="12"/>
+      <c r="AA97" s="12"/>
+      <c r="AB97" s="12"/>
+      <c r="AC97" s="12"/>
+      <c r="AD97" s="12"/>
+      <c r="AE97" s="12"/>
+      <c r="AF97" s="12"/>
+      <c r="AG97" s="12"/>
+      <c r="AH97" s="12"/>
+      <c r="AI97" s="12"/>
+      <c r="AJ97" s="12"/>
+      <c r="AK97" s="12"/>
+      <c r="AL97" s="12"/>
+      <c r="AM97" s="12"/>
+      <c r="AN97" s="12"/>
+      <c r="AO97" s="12"/>
+      <c r="AP97" s="12"/>
+      <c r="AQ97" s="12"/>
+      <c r="AR97" s="12"/>
+      <c r="AS97" s="12"/>
+      <c r="AT97" s="12"/>
+      <c r="AU97" s="12"/>
+      <c r="AV97" s="12"/>
+      <c r="AW97" s="12"/>
     </row>
     <row r="98" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B98" s="9"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="10"/>
-      <c r="H98" s="10"/>
-      <c r="I98" s="10"/>
-      <c r="J98" s="10"/>
-      <c r="K98" s="10"/>
-      <c r="L98" s="10"/>
-      <c r="M98" s="10"/>
-      <c r="N98" s="10"/>
-      <c r="O98" s="10"/>
-      <c r="P98" s="10"/>
-      <c r="Q98" s="10"/>
-      <c r="R98" s="10"/>
-      <c r="S98" s="10"/>
-      <c r="T98" s="10"/>
-      <c r="U98" s="10"/>
-      <c r="V98" s="10"/>
-      <c r="W98" s="10"/>
-      <c r="X98" s="10"/>
-      <c r="Y98" s="10"/>
-      <c r="Z98" s="10"/>
-      <c r="AA98" s="10"/>
-      <c r="AB98" s="10"/>
-      <c r="AC98" s="10"/>
-      <c r="AD98" s="10"/>
-      <c r="AE98" s="10"/>
-      <c r="AF98" s="10"/>
-      <c r="AG98" s="10"/>
-      <c r="AH98" s="10"/>
-      <c r="AI98" s="10"/>
-      <c r="AJ98" s="10"/>
-      <c r="AK98" s="10"/>
-      <c r="AL98" s="10"/>
-      <c r="AM98" s="10"/>
-      <c r="AN98" s="10"/>
-      <c r="AO98" s="10"/>
-      <c r="AP98" s="10"/>
-      <c r="AQ98" s="10"/>
-      <c r="AR98" s="10"/>
-      <c r="AS98" s="10"/>
-      <c r="AT98" s="10"/>
-      <c r="AU98" s="10"/>
-      <c r="AV98" s="10"/>
-      <c r="AW98" s="11"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+      <c r="O98" s="12"/>
+      <c r="P98" s="12"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="12"/>
+      <c r="S98" s="12"/>
+      <c r="T98" s="12"/>
+      <c r="U98" s="12"/>
+      <c r="V98" s="12"/>
+      <c r="W98" s="12"/>
+      <c r="X98" s="12"/>
+      <c r="Y98" s="12"/>
+      <c r="Z98" s="12"/>
+      <c r="AA98" s="12"/>
+      <c r="AB98" s="12"/>
+      <c r="AC98" s="12"/>
+      <c r="AD98" s="12"/>
+      <c r="AE98" s="12"/>
+      <c r="AF98" s="12"/>
+      <c r="AG98" s="12"/>
+      <c r="AH98" s="12"/>
+      <c r="AI98" s="12"/>
+      <c r="AJ98" s="12"/>
+      <c r="AK98" s="12"/>
+      <c r="AL98" s="12"/>
+      <c r="AM98" s="12"/>
+      <c r="AN98" s="12"/>
+      <c r="AO98" s="12"/>
+      <c r="AP98" s="12"/>
+      <c r="AQ98" s="12"/>
+      <c r="AR98" s="12"/>
+      <c r="AS98" s="12"/>
+      <c r="AT98" s="12"/>
+      <c r="AU98" s="12"/>
+      <c r="AV98" s="12"/>
+      <c r="AW98" s="12"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -7853,8 +9269,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId4" name="BtnLoadAA">
+        <control shapeId="1036" r:id="rId4" name="BtnUpdateAA">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>21</xdr:col>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>29</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1036" r:id="rId4" name="BtnUpdateAA"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1034" r:id="rId6" name="BtnLoadAA">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -7873,13 +9314,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId4" name="BtnLoadAA"/>
+        <control shapeId="1034" r:id="rId6" name="BtnLoadAA"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId6" name="TxtReviewDate">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1033" r:id="rId8" name="TxtReviewDate">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>50</xdr:col>
@@ -7898,13 +9339,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1033" r:id="rId6" name="TxtReviewDate"/>
+        <control shapeId="1033" r:id="rId8" name="TxtReviewDate"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId8" name="CmoRole">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="1032" r:id="rId10" name="CmoRole">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>50</xdr:col>
@@ -7923,12 +9364,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1032" r:id="rId8" name="CmoRole"/>
+        <control shapeId="1032" r:id="rId10" name="CmoRole"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId10" name="CmoContract">
+        <control shapeId="1031" r:id="rId12" name="CmoContract">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
@@ -7948,13 +9389,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1031" r:id="rId10" name="CmoContract"/>
+        <control shapeId="1031" r:id="rId12" name="CmoContract"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId12" name="TxtTemplateDate">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1030" r:id="rId13" name="TxtTemplateDate">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>50</xdr:col>
@@ -7973,13 +9414,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId12" name="TxtTemplateDate"/>
+        <control shapeId="1030" r:id="rId13" name="TxtTemplateDate"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId13" name="TxtNoWeeks">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+        <control shapeId="1029" r:id="rId15" name="TxtNoWeeks">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -7998,13 +9439,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId13" name="TxtNoWeeks"/>
+        <control shapeId="1029" r:id="rId15" name="TxtNoWeeks"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId15" name="TxtName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1028" r:id="rId17" name="TxtName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8023,13 +9464,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId15" name="TxtName"/>
+        <control shapeId="1028" r:id="rId17" name="TxtName"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId16" name="TxtCrewNo">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1027" r:id="rId19" name="TxtCrewNo">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8048,13 +9489,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId16" name="TxtCrewNo"/>
+        <control shapeId="1027" r:id="rId19" name="TxtCrewNo"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId17" name="CmoStation1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+        <control shapeId="1025" r:id="rId21" name="CmoStation1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8073,13 +9514,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId17" name="CmoStation1"/>
+        <control shapeId="1025" r:id="rId21" name="CmoStation1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId19" name="CmoStation2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+        <control shapeId="1026" r:id="rId22" name="CmoStation2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>49</xdr:col>
@@ -8098,13 +9539,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId19" name="CmoStation2"/>
+        <control shapeId="1026" r:id="rId22" name="CmoStation2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId21" name="BtnNewAA">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
+        <control shapeId="1035" r:id="rId24" name="BtnNewAA">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>13</xdr:col>
@@ -8123,7 +9564,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1035" r:id="rId21" name="BtnNewAA"/>
+        <control shapeId="1035" r:id="rId24" name="BtnNewAA"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>